<commit_message>
updated data & figures
</commit_message>
<xml_diff>
--- a/Data/Example1 - edited.xlsx
+++ b/Data/Example1 - edited.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lukem\Dropbox\FSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HowToAttributeCredit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD79734-D3BF-442B-9C83-BACB0D715DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01F63EE-D6F6-4A9C-A0E2-B7547B44CE11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -786,11 +786,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1:$O$1</c:f>
+              <c:f>Sheet1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PageRank Indegree Katz Eigenvector</c:v>
+                  <c:v>PageRank</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1348,6 +1348,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indegree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1901,6 +1912,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Katz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -2454,6 +2476,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eigenvector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -5196,8 +5229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W175"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11:T11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R175" sqref="R175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13569,7 +13602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97002E43-40C3-4689-9E9F-A0E1A4F6F6A4}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="B2:E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>